<commit_message>
Updating user path : AK
</commit_message>
<xml_diff>
--- a/target/classes/Resources/ReadData.xlsx
+++ b/target/classes/Resources/ReadData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>FirstRow</t>
   </si>
@@ -416,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -528,6 +528,28 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>